<commit_message>
use srl instead of div
</commit_message>
<xml_diff>
--- a/CSCI-361FinalProject/running_time.xlsx
+++ b/CSCI-361FinalProject/running_time.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>Instruction type</t>
   </si>
@@ -65,6 +65,15 @@
   </si>
   <si>
     <t>MARS Tool Output</t>
+  </si>
+  <si>
+    <t>Percent Improvement</t>
+  </si>
+  <si>
+    <t>Original Running Time</t>
+  </si>
+  <si>
+    <t>Goal Running Time</t>
   </si>
 </sst>
 </file>
@@ -134,12 +143,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -444,22 +454,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F16"/>
+  <dimension ref="A2:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
@@ -469,12 +480,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
@@ -491,145 +502,207 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>1</v>
       </c>
       <c r="B6">
-        <v>4319</v>
+        <v>3175</v>
       </c>
       <c r="D6">
         <f>B6</f>
-        <v>4319</v>
+        <v>3175</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
       <c r="F6">
         <f>D6*E6</f>
-        <v>4319</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3175</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>2</v>
       </c>
       <c r="B7">
-        <v>298</v>
+        <v>226</v>
       </c>
       <c r="D7">
         <f>B7</f>
-        <v>298</v>
+        <v>226</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
       <c r="F7">
         <f>D7*E7</f>
-        <v>298</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>3</v>
       </c>
       <c r="B8">
-        <v>1166</v>
+        <v>871</v>
       </c>
       <c r="D8">
         <f>B8</f>
-        <v>1166</v>
+        <v>871</v>
       </c>
       <c r="E8">
         <v>2</v>
       </c>
       <c r="F8">
         <f>D8*E8</f>
-        <v>2332</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1742</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>4</v>
       </c>
       <c r="B9">
-        <v>820</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>5</v>
       </c>
       <c r="B10">
-        <v>1682</v>
+        <v>779</v>
       </c>
       <c r="D10">
         <f>B10-(B14+B15-B9)</f>
-        <v>1590</v>
+        <v>687</v>
       </c>
       <c r="E10">
         <v>5</v>
       </c>
       <c r="F10">
         <f>D10*E10</f>
-        <v>7950</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3435</v>
+      </c>
+      <c r="H10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H11">
+        <v>31961</v>
+      </c>
+      <c r="K11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J12" s="5">
+        <v>1</v>
+      </c>
+      <c r="K12">
+        <f>H11/6</f>
+        <v>5326.833333333333</v>
+      </c>
+      <c r="L12">
+        <f>((H11-K12)/H11)*100</f>
+        <v>83.333333333333343</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J13" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="K13">
+        <f>H11/5</f>
+        <v>6392.2</v>
+      </c>
+      <c r="L13">
+        <f>((H11-K13)/H11)*100</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>9</v>
       </c>
       <c r="B14">
-        <v>511</v>
+        <v>435</v>
       </c>
       <c r="D14">
         <f>B14</f>
-        <v>511</v>
+        <v>435</v>
       </c>
       <c r="E14">
         <v>2</v>
       </c>
       <c r="F14">
         <f>D14*E14</f>
-        <v>1022</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>870</v>
+      </c>
+      <c r="J14" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="K14">
+        <f>H11/4</f>
+        <v>7990.25</v>
+      </c>
+      <c r="L14">
+        <f>((H11-K14)/H11)*100</f>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>10</v>
       </c>
       <c r="B15">
-        <v>401</v>
+        <v>287</v>
       </c>
       <c r="D15">
         <f>B15</f>
-        <v>401</v>
+        <v>287</v>
       </c>
       <c r="E15">
         <v>40</v>
       </c>
       <c r="F15">
         <f>D15*E15</f>
-        <v>16040</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+        <v>11480</v>
+      </c>
+      <c r="H15" t="s">
+        <v>17</v>
+      </c>
+      <c r="J15" s="5">
+        <v>0.7</v>
+      </c>
+      <c r="K15">
+        <f>H11/2</f>
+        <v>15980.5</v>
+      </c>
+      <c r="L15">
+        <f>((H11-K15)/H11)*100</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="18" x14ac:dyDescent="0.35">
       <c r="F16" s="4">
         <f>SUM(F6:F15)</f>
-        <v>31961</v>
+        <v>20928</v>
+      </c>
+      <c r="H16">
+        <f>((H11-F16)/H11)*100</f>
+        <v>34.520196489471545</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
only interact with even numbers
</commit_message>
<xml_diff>
--- a/CSCI-361FinalProject/running_time.xlsx
+++ b/CSCI-361FinalProject/running_time.xlsx
@@ -456,8 +456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -507,18 +507,18 @@
         <v>1</v>
       </c>
       <c r="B6">
-        <v>3175</v>
+        <v>1911</v>
       </c>
       <c r="D6">
         <f>B6</f>
-        <v>3175</v>
+        <v>1911</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
       <c r="F6">
         <f>D6*E6</f>
-        <v>3175</v>
+        <v>1911</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
@@ -526,18 +526,18 @@
         <v>2</v>
       </c>
       <c r="B7">
-        <v>226</v>
+        <v>162</v>
       </c>
       <c r="D7">
         <f>B7</f>
-        <v>226</v>
+        <v>162</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
       <c r="F7">
         <f>D7*E7</f>
-        <v>226</v>
+        <v>162</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
@@ -545,18 +545,18 @@
         <v>3</v>
       </c>
       <c r="B8">
-        <v>871</v>
+        <v>506</v>
       </c>
       <c r="D8">
         <f>B8</f>
-        <v>871</v>
+        <v>506</v>
       </c>
       <c r="E8">
         <v>2</v>
       </c>
       <c r="F8">
         <f>D8*E8</f>
-        <v>1742</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
@@ -564,7 +564,7 @@
         <v>4</v>
       </c>
       <c r="B9">
-        <v>630</v>
+        <v>365</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
@@ -572,18 +572,18 @@
         <v>5</v>
       </c>
       <c r="B10">
-        <v>779</v>
+        <v>507</v>
       </c>
       <c r="D10">
         <f>B10-(B14+B15-B9)</f>
-        <v>687</v>
+        <v>415</v>
       </c>
       <c r="E10">
         <v>5</v>
       </c>
       <c r="F10">
         <f>D10*E10</f>
-        <v>3435</v>
+        <v>2075</v>
       </c>
       <c r="H10" t="s">
         <v>18</v>
@@ -637,18 +637,18 @@
         <v>9</v>
       </c>
       <c r="B14">
-        <v>435</v>
+        <v>193</v>
       </c>
       <c r="D14">
         <f>B14</f>
-        <v>435</v>
+        <v>193</v>
       </c>
       <c r="E14">
         <v>2</v>
       </c>
       <c r="F14">
         <f>D14*E14</f>
-        <v>870</v>
+        <v>386</v>
       </c>
       <c r="J14" s="5">
         <v>0.8</v>
@@ -667,18 +667,18 @@
         <v>10</v>
       </c>
       <c r="B15">
-        <v>287</v>
+        <v>264</v>
       </c>
       <c r="D15">
         <f>B15</f>
-        <v>287</v>
+        <v>264</v>
       </c>
       <c r="E15">
         <v>40</v>
       </c>
       <c r="F15">
         <f>D15*E15</f>
-        <v>11480</v>
+        <v>10560</v>
       </c>
       <c r="H15" t="s">
         <v>17</v>
@@ -698,11 +698,11 @@
     <row r="16" spans="1:12" ht="18" x14ac:dyDescent="0.35">
       <c r="F16" s="4">
         <f>SUM(F6:F15)</f>
-        <v>20928</v>
+        <v>16106</v>
       </c>
       <c r="H16">
         <f>((H11-F16)/H11)*100</f>
-        <v>34.520196489471545</v>
+        <v>49.607333938237225</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
track dat stack pointer instead of recalculating
</commit_message>
<xml_diff>
--- a/CSCI-361FinalProject/running_time.xlsx
+++ b/CSCI-361FinalProject/running_time.xlsx
@@ -456,8 +456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="D2" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -507,18 +507,18 @@
         <v>1</v>
       </c>
       <c r="B6">
-        <v>1911</v>
+        <v>1019</v>
       </c>
       <c r="D6">
         <f>B6</f>
-        <v>1911</v>
+        <v>1019</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
       <c r="F6">
         <f>D6*E6</f>
-        <v>1911</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
@@ -526,18 +526,18 @@
         <v>2</v>
       </c>
       <c r="B7">
-        <v>162</v>
+        <v>79</v>
       </c>
       <c r="D7">
         <f>B7</f>
-        <v>162</v>
+        <v>79</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
       <c r="F7">
         <f>D7*E7</f>
-        <v>162</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
@@ -545,18 +545,18 @@
         <v>3</v>
       </c>
       <c r="B8">
-        <v>506</v>
+        <v>423</v>
       </c>
       <c r="D8">
         <f>B8</f>
-        <v>506</v>
+        <v>423</v>
       </c>
       <c r="E8">
         <v>2</v>
       </c>
       <c r="F8">
         <f>D8*E8</f>
-        <v>1012</v>
+        <v>846</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
@@ -564,7 +564,7 @@
         <v>4</v>
       </c>
       <c r="B9">
-        <v>365</v>
+        <v>277</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
@@ -572,18 +572,18 @@
         <v>5</v>
       </c>
       <c r="B10">
-        <v>507</v>
+        <v>424</v>
       </c>
       <c r="D10">
         <f>B10-(B14+B15-B9)</f>
-        <v>415</v>
+        <v>332</v>
       </c>
       <c r="E10">
         <v>5</v>
       </c>
       <c r="F10">
         <f>D10*E10</f>
-        <v>2075</v>
+        <v>1660</v>
       </c>
       <c r="H10" t="s">
         <v>18</v>
@@ -637,18 +637,18 @@
         <v>9</v>
       </c>
       <c r="B14">
-        <v>193</v>
+        <v>171</v>
       </c>
       <c r="D14">
         <f>B14</f>
-        <v>193</v>
+        <v>171</v>
       </c>
       <c r="E14">
         <v>2</v>
       </c>
       <c r="F14">
         <f>D14*E14</f>
-        <v>386</v>
+        <v>342</v>
       </c>
       <c r="J14" s="5">
         <v>0.8</v>
@@ -667,18 +667,18 @@
         <v>10</v>
       </c>
       <c r="B15">
-        <v>264</v>
+        <v>198</v>
       </c>
       <c r="D15">
         <f>B15</f>
-        <v>264</v>
+        <v>198</v>
       </c>
       <c r="E15">
         <v>40</v>
       </c>
       <c r="F15">
         <f>D15*E15</f>
-        <v>10560</v>
+        <v>7920</v>
       </c>
       <c r="H15" t="s">
         <v>17</v>
@@ -698,11 +698,11 @@
     <row r="16" spans="1:12" ht="18" x14ac:dyDescent="0.35">
       <c r="F16" s="4">
         <f>SUM(F6:F15)</f>
-        <v>16106</v>
+        <v>11866</v>
       </c>
       <c r="H16">
         <f>((H11-F16)/H11)*100</f>
-        <v>49.607333938237225</v>
+        <v>62.873502080660806</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remove even elements from mem
</commit_message>
<xml_diff>
--- a/CSCI-361FinalProject/running_time.xlsx
+++ b/CSCI-361FinalProject/running_time.xlsx
@@ -456,8 +456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D2" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="E2" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -637,18 +637,18 @@
         <v>9</v>
       </c>
       <c r="B14">
-        <v>171</v>
+        <v>227</v>
       </c>
       <c r="D14">
         <f>B14</f>
-        <v>171</v>
+        <v>227</v>
       </c>
       <c r="E14">
         <v>2</v>
       </c>
       <c r="F14">
         <f>D14*E14</f>
-        <v>342</v>
+        <v>454</v>
       </c>
       <c r="J14" s="5">
         <v>0.8</v>
@@ -667,18 +667,18 @@
         <v>10</v>
       </c>
       <c r="B15">
-        <v>198</v>
+        <v>142</v>
       </c>
       <c r="D15">
         <f>B15</f>
-        <v>198</v>
+        <v>142</v>
       </c>
       <c r="E15">
         <v>40</v>
       </c>
       <c r="F15">
         <f>D15*E15</f>
-        <v>7920</v>
+        <v>5680</v>
       </c>
       <c r="H15" t="s">
         <v>17</v>
@@ -698,11 +698,11 @@
     <row r="16" spans="1:12" ht="18" x14ac:dyDescent="0.35">
       <c r="F16" s="4">
         <f>SUM(F6:F15)</f>
-        <v>11866</v>
+        <v>9738</v>
       </c>
       <c r="H16">
         <f>((H11-F16)/H11)*100</f>
-        <v>62.873502080660806</v>
+        <v>69.531616657801692</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
store half words instead of words
</commit_message>
<xml_diff>
--- a/CSCI-361FinalProject/running_time.xlsx
+++ b/CSCI-361FinalProject/running_time.xlsx
@@ -456,8 +456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E2" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -637,18 +637,18 @@
         <v>9</v>
       </c>
       <c r="B14">
-        <v>227</v>
+        <v>290</v>
       </c>
       <c r="D14">
         <f>B14</f>
-        <v>227</v>
+        <v>290</v>
       </c>
       <c r="E14">
         <v>2</v>
       </c>
       <c r="F14">
         <f>D14*E14</f>
-        <v>454</v>
+        <v>580</v>
       </c>
       <c r="J14" s="5">
         <v>0.8</v>
@@ -667,18 +667,18 @@
         <v>10</v>
       </c>
       <c r="B15">
-        <v>142</v>
+        <v>79</v>
       </c>
       <c r="D15">
         <f>B15</f>
-        <v>142</v>
+        <v>79</v>
       </c>
       <c r="E15">
         <v>40</v>
       </c>
       <c r="F15">
         <f>D15*E15</f>
-        <v>5680</v>
+        <v>3160</v>
       </c>
       <c r="H15" t="s">
         <v>17</v>
@@ -698,11 +698,11 @@
     <row r="16" spans="1:12" ht="18" x14ac:dyDescent="0.35">
       <c r="F16" s="4">
         <f>SUM(F6:F15)</f>
-        <v>9738</v>
+        <v>7344</v>
       </c>
       <c r="H16">
         <f>((H11-F16)/H11)*100</f>
-        <v>69.531616657801692</v>
+        <v>77.021995557085205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
store bytes instead of half word
</commit_message>
<xml_diff>
--- a/CSCI-361FinalProject/running_time.xlsx
+++ b/CSCI-361FinalProject/running_time.xlsx
@@ -456,8 +456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -637,18 +637,18 @@
         <v>9</v>
       </c>
       <c r="B14">
-        <v>290</v>
+        <v>361</v>
       </c>
       <c r="D14">
         <f>B14</f>
-        <v>290</v>
+        <v>361</v>
       </c>
       <c r="E14">
         <v>2</v>
       </c>
       <c r="F14">
         <f>D14*E14</f>
-        <v>580</v>
+        <v>722</v>
       </c>
       <c r="J14" s="5">
         <v>0.8</v>
@@ -667,18 +667,18 @@
         <v>10</v>
       </c>
       <c r="B15">
-        <v>79</v>
+        <v>8</v>
       </c>
       <c r="D15">
         <f>B15</f>
-        <v>79</v>
+        <v>8</v>
       </c>
       <c r="E15">
         <v>40</v>
       </c>
       <c r="F15">
         <f>D15*E15</f>
-        <v>3160</v>
+        <v>320</v>
       </c>
       <c r="H15" t="s">
         <v>17</v>
@@ -698,11 +698,11 @@
     <row r="16" spans="1:12" ht="18" x14ac:dyDescent="0.35">
       <c r="F16" s="4">
         <f>SUM(F6:F15)</f>
-        <v>7344</v>
+        <v>4646</v>
       </c>
       <c r="H16">
         <f>((H11-F16)/H11)*100</f>
-        <v>77.021995557085205</v>
+        <v>85.463533681674548</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor tweaks for another 1.5%
</commit_message>
<xml_diff>
--- a/CSCI-361FinalProject/running_time.xlsx
+++ b/CSCI-361FinalProject/running_time.xlsx
@@ -457,7 +457,7 @@
   <dimension ref="A2:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -507,18 +507,18 @@
         <v>1</v>
       </c>
       <c r="B6">
-        <v>1019</v>
+        <v>816</v>
       </c>
       <c r="D6">
         <f>B6</f>
-        <v>1019</v>
+        <v>816</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
       <c r="F6">
         <f>D6*E6</f>
-        <v>1019</v>
+        <v>816</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
@@ -572,18 +572,18 @@
         <v>5</v>
       </c>
       <c r="B10">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D10">
         <f>B10-(B14+B15-B9)</f>
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="E10">
         <v>5</v>
       </c>
       <c r="F10">
         <f>D10*E10</f>
-        <v>1660</v>
+        <v>1650</v>
       </c>
       <c r="H10" t="s">
         <v>18</v>
@@ -698,11 +698,11 @@
     <row r="16" spans="1:12" ht="18" x14ac:dyDescent="0.35">
       <c r="F16" s="4">
         <f>SUM(F6:F15)</f>
-        <v>4646</v>
+        <v>4433</v>
       </c>
       <c r="H16">
         <f>((H11-F16)/H11)*100</f>
-        <v>85.463533681674548</v>
+        <v>86.12997090203686</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
triple unrolled init loop and comments
</commit_message>
<xml_diff>
--- a/CSCI-361FinalProject/running_time.xlsx
+++ b/CSCI-361FinalProject/running_time.xlsx
@@ -456,8 +456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -507,18 +507,18 @@
         <v>1</v>
       </c>
       <c r="B6">
-        <v>816</v>
+        <v>708</v>
       </c>
       <c r="D6">
         <f>B6</f>
-        <v>816</v>
+        <v>708</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
       <c r="F6">
         <f>D6*E6</f>
-        <v>816</v>
+        <v>708</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
@@ -545,18 +545,18 @@
         <v>3</v>
       </c>
       <c r="B8">
-        <v>423</v>
+        <v>355</v>
       </c>
       <c r="D8">
         <f>B8</f>
-        <v>423</v>
+        <v>355</v>
       </c>
       <c r="E8">
         <v>2</v>
       </c>
       <c r="F8">
         <f>D8*E8</f>
-        <v>846</v>
+        <v>710</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
@@ -572,18 +572,18 @@
         <v>5</v>
       </c>
       <c r="B10">
-        <v>422</v>
+        <v>350</v>
       </c>
       <c r="D10">
         <f>B10-(B14+B15-B9)</f>
-        <v>330</v>
+        <v>262</v>
       </c>
       <c r="E10">
         <v>5</v>
       </c>
       <c r="F10">
         <f>D10*E10</f>
-        <v>1650</v>
+        <v>1310</v>
       </c>
       <c r="H10" t="s">
         <v>18</v>
@@ -637,18 +637,18 @@
         <v>9</v>
       </c>
       <c r="B14">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="D14">
         <f>B14</f>
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="E14">
         <v>2</v>
       </c>
       <c r="F14">
         <f>D14*E14</f>
-        <v>722</v>
+        <v>714</v>
       </c>
       <c r="J14" s="5">
         <v>0.8</v>
@@ -698,11 +698,11 @@
     <row r="16" spans="1:12" ht="18" x14ac:dyDescent="0.35">
       <c r="F16" s="4">
         <f>SUM(F6:F15)</f>
-        <v>4433</v>
+        <v>3841</v>
       </c>
       <c r="H16">
         <f>((H11-F16)/H11)*100</f>
-        <v>86.12997090203686</v>
+        <v>87.982228340790343</v>
       </c>
     </row>
   </sheetData>

</xml_diff>